<commit_message>
Re-run all analysis with corrected file names for boxplots.
</commit_message>
<xml_diff>
--- a/output/20221121/tables/effort/betas_index.xlsx
+++ b/output/20221121/tables/effort/betas_index.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1463" uniqueCount="22">
   <si>
     <t>Outcome</t>
   </si>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -123,8 +123,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">

</xml_diff>